<commit_message>
Second GIT commit, still testing how GIT works with pycharm.
</commit_message>
<xml_diff>
--- a/MoneyWizsDocs/Tasks_MoneyWizs.xlsx
+++ b/MoneyWizsDocs/Tasks_MoneyWizs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -64,6 +64,51 @@
   </si>
   <si>
     <t>26/3/2017</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>Basic Blog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27/3/2017 </t>
+  </si>
+  <si>
+    <t>Basic Authentication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/3/2017 </t>
+  </si>
+  <si>
+    <t>Basic Forum</t>
+  </si>
+  <si>
+    <t>30/3/2017</t>
+  </si>
+  <si>
+    <t>Basic searching</t>
+  </si>
+  <si>
+    <t>28/3/2017</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Basic Registration</t>
+  </si>
+  <si>
+    <t>27/3/2017</t>
+  </si>
+  <si>
+    <t>Yet to start</t>
   </si>
 </sst>
 </file>
@@ -87,15 +132,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -103,13 +160,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,21 +499,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.08984375" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
-    <col min="4" max="4" width="21.36328125" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" customWidth="1"/>
-    <col min="6" max="6" width="16.1796875" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="1" max="1" width="30.08984375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.36328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
@@ -465,45 +541,151 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>